<commit_message>
testes debug e agent
</commit_message>
<xml_diff>
--- a/docs/validacao.xlsx
+++ b/docs/validacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TJRS\PythonProjects\temas_llm\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECA02C8-675E-41EB-A838-BE7CF9C9B89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712AD699-40EA-498A-ACFA-CBB41F55E5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9075" yWindow="705" windowWidth="26565" windowHeight="14550" xr2:uid="{737D3783-D5B0-4DB4-9674-1F6685FBF5B9}"/>
   </bookViews>
@@ -36,20 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Arquivo</t>
   </si>
   <si>
-    <t>GT</t>
-  </si>
-  <si>
     <t>BGE</t>
   </si>
   <si>
-    <t>SBERT</t>
-  </si>
-  <si>
     <t>685 STJ</t>
   </si>
   <si>
@@ -90,6 +84,21 @@
   </si>
   <si>
     <t>Ok na busca (247) - OK no LLM</t>
+  </si>
+  <si>
+    <t>SBERT distiluse</t>
+  </si>
+  <si>
+    <t>Fail na busca - Fail no LLM</t>
+  </si>
+  <si>
+    <t>SBERT paraphrase MiniLM</t>
+  </si>
+  <si>
+    <t>SBERT paraphrase mpnet</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
   </si>
 </sst>
 </file>
@@ -470,100 +479,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36909E21-2460-4756-8850-A25B201FF054}">
-  <dimension ref="C2:F10"/>
+  <dimension ref="C2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
     </row>
   </sheetData>

</xml_diff>